<commit_message>
- Fix Data - Fix Customer Write Cell - Added Product Update - Added Product Delete
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/CMPG323 EcoPower Logistics Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nttlimited-my.sharepoint.com/personal/jacqui_muller_dimensiondata_com/Documents/NWU/2023 CMPG323/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NWU 2023 BSC IT\2nd Semester\CMPG323 - IT DEVELOPMENTS\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{5546F926-6C85-4EAE-890A-D0833008B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B224C2EE-D72C-413C-83C8-0FBC3DD6E173}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388DB056-EF28-49CD-A599-D50F0AE4FB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15225" yWindow="1815" windowWidth="13500" windowHeight="14160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -1715,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>